<commit_message>
Tạo file react + install package
</commit_message>
<xml_diff>
--- a/Document/template_task.xlsx
+++ b/Document/template_task.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sarah\Documents\Frontend\HW\Airbnb\Document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67B8EA0C-807B-40F9-90AD-AA1BF5578DB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6F3D72C-75EF-4CFD-807F-C7E718074953}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="32">
   <si>
     <t>Tasks Name</t>
   </si>
@@ -98,6 +98,45 @@
   </si>
   <si>
     <t>Nguyên Phi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Homepage </t>
+  </si>
+  <si>
+    <t>Đăng nhập + Đăng ký + upload ảnh</t>
+  </si>
+  <si>
+    <t>Danh sách phòng ở</t>
+  </si>
+  <si>
+    <t>Chi tiết phòng ở + Danh sách tiện ích</t>
+  </si>
+  <si>
+    <t>Xác nhận và đặt chỗ + Đăng xuất</t>
+  </si>
+  <si>
+    <t>Chỉnh sửa thông tin tài khoản</t>
+  </si>
+  <si>
+    <t>Lịch sử đặt phòng + Chi tiết vé</t>
+  </si>
+  <si>
+    <t>Homepage admin</t>
+  </si>
+  <si>
+    <t>Quản lý người dùng</t>
+  </si>
+  <si>
+    <t>Quản lý vị trí</t>
+  </si>
+  <si>
+    <t>Quản lý phòng cho thuê</t>
+  </si>
+  <si>
+    <t>Quản lý đánh giá</t>
+  </si>
+  <si>
+    <t>Quản lý vé</t>
   </si>
 </sst>
 </file>
@@ -622,12 +661,12 @@
   <dimension ref="A1:J985"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" outlineLevelRow="2" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.5" customWidth="1"/>
+    <col min="1" max="1" width="23.9140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.08203125" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="7.6640625" customWidth="1"/>
     <col min="5" max="5" width="10.25" customWidth="1"/>
@@ -838,11 +877,17 @@
       <c r="J7" s="22"/>
     </row>
     <row r="8" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="7"/>
-      <c r="B8" s="8"/>
+      <c r="A8" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="25">
+        <v>44623</v>
+      </c>
       <c r="C8" s="8"/>
       <c r="D8" s="9"/>
-      <c r="E8" s="10"/>
+      <c r="E8" s="10" t="s">
+        <v>17</v>
+      </c>
       <c r="F8" s="11"/>
       <c r="G8" s="8"/>
       <c r="H8" s="12"/>
@@ -850,7 +895,9 @@
       <c r="J8" s="13"/>
     </row>
     <row r="9" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="7"/>
+      <c r="A9" s="7" t="s">
+        <v>20</v>
+      </c>
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
       <c r="D9" s="9"/>
@@ -862,7 +909,9 @@
       <c r="J9" s="13"/>
     </row>
     <row r="10" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="7"/>
+      <c r="A10" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
       <c r="D10" s="9"/>
@@ -874,7 +923,9 @@
       <c r="J10" s="13"/>
     </row>
     <row r="11" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="7"/>
+      <c r="A11" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
       <c r="D11" s="9"/>
@@ -886,7 +937,9 @@
       <c r="J11" s="13"/>
     </row>
     <row r="12" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="7"/>
+      <c r="A12" s="7" t="s">
+        <v>23</v>
+      </c>
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
       <c r="D12" s="9"/>
@@ -898,7 +951,9 @@
       <c r="J12" s="13"/>
     </row>
     <row r="13" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="7"/>
+      <c r="A13" s="7" t="s">
+        <v>24</v>
+      </c>
       <c r="B13" s="8"/>
       <c r="C13" s="8"/>
       <c r="D13" s="9"/>
@@ -909,25 +964,116 @@
       <c r="I13" s="10"/>
       <c r="J13" s="13"/>
     </row>
-    <row r="14" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="15" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="16" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="17" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="18" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="20" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="21" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="22" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="24" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="25" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="27" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="28" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="29" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="30" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="31" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="32" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="16"/>
+      <c r="J14" s="13"/>
+    </row>
+    <row r="15" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="11"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="16"/>
+      <c r="J15" s="13"/>
+    </row>
+    <row r="16" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="11"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="16"/>
+      <c r="J16" s="13"/>
+    </row>
+    <row r="17" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="16"/>
+      <c r="J17" s="13"/>
+    </row>
+    <row r="18" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" s="11"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="16"/>
+      <c r="J18" s="13"/>
+    </row>
+    <row r="19" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="16"/>
+      <c r="J19" s="13"/>
+    </row>
+    <row r="20" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" s="11"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="16"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="16"/>
+      <c r="J20" s="13"/>
+    </row>
+    <row r="21" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="22" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="23" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="24" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="25" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="26" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="27" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="28" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="29" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="30" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="31" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="32" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="33" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="34" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="35" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1882,7 +2028,7 @@
     <row r="984" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="985" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <conditionalFormatting sqref="D2 D4:D13 H4:H13">
+  <conditionalFormatting sqref="D2 D4:D20 H4:H20">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>

</xml_diff>

<commit_message>
fix bug and done XacNhan
</commit_message>
<xml_diff>
--- a/Document/template_task.xlsx
+++ b/Document/template_task.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sarah\Documents\Frontend\HW\Airbnb\Document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A68453B-3F56-404F-A08D-9EABE82B57D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0484A5F4-B1FF-48BF-9FE7-C540671910FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="32">
   <si>
     <t>Tasks Name</t>
   </si>
@@ -146,7 +146,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -172,10 +172,6 @@
     <font>
       <sz val="9"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="9"/>
       <name val="Calibri"/>
     </font>
     <font>
@@ -223,7 +219,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -321,24 +317,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -402,19 +385,13 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="2" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="2" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -661,7 +638,7 @@
   <dimension ref="A1:J985"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.69921875" defaultRowHeight="15" customHeight="1" outlineLevelRow="2" x14ac:dyDescent="0.25"/>
@@ -714,28 +691,28 @@
       <c r="A2" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="25">
+      <c r="B2" s="23">
         <v>44620</v>
       </c>
-      <c r="C2" s="26">
+      <c r="C2" s="24">
         <v>44623</v>
       </c>
       <c r="D2" s="9">
         <v>0.6</v>
       </c>
-      <c r="E2" s="27" t="s">
+      <c r="E2" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="25">
+      <c r="F2" s="23">
         <v>44622</v>
       </c>
-      <c r="G2" s="25">
+      <c r="G2" s="23">
         <v>44624</v>
       </c>
       <c r="H2" s="12">
         <v>1</v>
       </c>
-      <c r="I2" s="27" t="s">
+      <c r="I2" s="25" t="s">
         <v>18</v>
       </c>
       <c r="J2" s="13"/>
@@ -882,10 +859,10 @@
       <c r="A8" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="25">
+      <c r="B8" s="23">
         <v>44623</v>
       </c>
-      <c r="C8" s="26">
+      <c r="C8" s="24">
         <v>44631</v>
       </c>
       <c r="D8" s="9">
@@ -904,10 +881,10 @@
       <c r="A9" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="25">
+      <c r="B9" s="23">
         <v>44626</v>
       </c>
-      <c r="C9" s="26">
+      <c r="C9" s="24">
         <v>44631</v>
       </c>
       <c r="D9" s="9">
@@ -926,10 +903,10 @@
       <c r="A10" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="25">
+      <c r="B10" s="23">
         <v>44632</v>
       </c>
-      <c r="C10" s="25">
+      <c r="C10" s="23">
         <v>44641</v>
       </c>
       <c r="D10" s="9">
@@ -948,16 +925,18 @@
       <c r="A11" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="25">
+      <c r="B11" s="23">
         <v>44641</v>
       </c>
-      <c r="C11" s="25">
+      <c r="C11" s="23">
         <v>44642</v>
       </c>
       <c r="D11" s="9">
         <v>0.6</v>
       </c>
-      <c r="E11" s="23"/>
+      <c r="E11" s="16" t="s">
+        <v>17</v>
+      </c>
       <c r="F11" s="11"/>
       <c r="G11" s="8"/>
       <c r="H11" s="12"/>
@@ -968,12 +947,18 @@
       <c r="A12" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="25">
+      <c r="B12" s="23">
         <v>44642</v>
       </c>
-      <c r="C12" s="8"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="24"/>
+      <c r="C12" s="23">
+        <v>44642</v>
+      </c>
+      <c r="D12" s="9">
+        <v>0.6</v>
+      </c>
+      <c r="E12" s="16" t="s">
+        <v>17</v>
+      </c>
       <c r="F12" s="11"/>
       <c r="G12" s="8"/>
       <c r="H12" s="12"/>

</xml_diff>